<commit_message>
add phonetic keyboard sign on keyman developer project
</commit_message>
<xml_diff>
--- a/Keyboard Project/mapping.xlsx
+++ b/Keyboard Project/mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Library/CloudStorage/GoogleDrive-mengthongoenggl@gmail.com/My Drive/KhmerSignWriting-Fingerspelling-Keyboard/Keyboard Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Keyboard_layouts_for_Cambodian_Fingerspelling\Keyboard Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40D3E06-729C-DB42-9305-0E7E6919A13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5723A8E-C8F1-42ED-AED4-BFF31750013C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17040" yWindow="500" windowWidth="22100" windowHeight="22460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="16410" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="178">
   <si>
     <t>N</t>
   </si>
@@ -45,304 +45,151 @@
     <t>ក</t>
   </si>
   <si>
-    <t>1D873</t>
-  </si>
-  <si>
     <t>ខ</t>
-  </si>
-  <si>
-    <t>1D806</t>
   </si>
   <si>
     <t>គ</t>
   </si>
   <si>
-    <t>1D816</t>
-  </si>
-  <si>
     <t>ឃ</t>
-  </si>
-  <si>
-    <t>1D8A4</t>
   </si>
   <si>
     <t>ង</t>
   </si>
   <si>
-    <t>1D842</t>
-  </si>
-  <si>
     <t>ច</t>
-  </si>
-  <si>
-    <t>1D845</t>
   </si>
   <si>
     <t>ឆ</t>
   </si>
   <si>
-    <t>1D850</t>
-  </si>
-  <si>
     <t>ជ</t>
-  </si>
-  <si>
-    <t>1D8B4</t>
   </si>
   <si>
     <t>ឈ</t>
   </si>
   <si>
-    <t>1D834</t>
-  </si>
-  <si>
     <t>ញ</t>
-  </si>
-  <si>
-    <t>1D893</t>
   </si>
   <si>
     <t>ដ</t>
   </si>
   <si>
-    <t>1D8CC</t>
-  </si>
-  <si>
     <t>ឋ</t>
-  </si>
-  <si>
-    <t>1D8C6</t>
   </si>
   <si>
     <t>ឌ</t>
   </si>
   <si>
-    <t>1D829</t>
-  </si>
-  <si>
     <t>ឍ</t>
-  </si>
-  <si>
-    <t>1D8BA</t>
   </si>
   <si>
     <t>ណ</t>
   </si>
   <si>
-    <t>1D8EF</t>
-  </si>
-  <si>
     <t>ត</t>
-  </si>
-  <si>
-    <t>1D84A</t>
   </si>
   <si>
     <t>ថ</t>
   </si>
   <si>
-    <t>1D89C</t>
-  </si>
-  <si>
     <t>ទ</t>
-  </si>
-  <si>
-    <t>1D83E</t>
   </si>
   <si>
     <t>ធ</t>
   </si>
   <si>
-    <t>1D844</t>
-  </si>
-  <si>
     <t>ន</t>
-  </si>
-  <si>
-    <t>1D895</t>
   </si>
   <si>
     <t>ប</t>
   </si>
   <si>
-    <t>1D8A0</t>
-  </si>
-  <si>
     <t>ផ</t>
-  </si>
-  <si>
-    <t>1D813</t>
   </si>
   <si>
     <t>ភ</t>
   </si>
   <si>
-    <t>1D846</t>
-  </si>
-  <si>
     <t>ព</t>
-  </si>
-  <si>
-    <t>1D828</t>
   </si>
   <si>
     <t>ម</t>
   </si>
   <si>
-    <t>1D848</t>
-  </si>
-  <si>
     <t>យ</t>
-  </si>
-  <si>
-    <t>1D88C</t>
   </si>
   <si>
     <t>រ</t>
   </si>
   <si>
-    <t>1D81D</t>
-  </si>
-  <si>
     <t>ល</t>
-  </si>
-  <si>
-    <t>1D82C</t>
   </si>
   <si>
     <t>វ</t>
   </si>
   <si>
-    <t>1D82E</t>
-  </si>
-  <si>
     <t>ស</t>
-  </si>
-  <si>
-    <t>1D896</t>
   </si>
   <si>
     <t>ហ</t>
   </si>
   <si>
-    <t>1D898</t>
-  </si>
-  <si>
-    <t>1D8C4</t>
-  </si>
-  <si>
     <t>អ</t>
-  </si>
-  <si>
-    <t>1D8B5</t>
   </si>
   <si>
     <t>ា</t>
   </si>
   <si>
-    <t>1D879</t>
-  </si>
-  <si>
     <t>ិ</t>
-  </si>
-  <si>
-    <t>1D85C</t>
   </si>
   <si>
     <t>ី</t>
   </si>
   <si>
-    <t>1D85E</t>
-  </si>
-  <si>
     <t>ឹ</t>
-  </si>
-  <si>
-    <t>1D809</t>
   </si>
   <si>
     <t>ឺ</t>
   </si>
   <si>
-    <t>1D819</t>
-  </si>
-  <si>
     <t>ុ</t>
-  </si>
-  <si>
-    <t>1D8C8</t>
   </si>
   <si>
     <t>ូ</t>
   </si>
   <si>
-    <t>1D8C9</t>
-  </si>
-  <si>
     <t>ួ</t>
-  </si>
-  <si>
-    <t>1D8CB</t>
   </si>
   <si>
     <t>ើ</t>
   </si>
   <si>
-    <t>1D87F</t>
-  </si>
-  <si>
     <t>ឿ</t>
-  </si>
-  <si>
-    <t>1D86A</t>
   </si>
   <si>
     <t>ៀ</t>
   </si>
   <si>
-    <t>1D869</t>
-  </si>
-  <si>
     <t>េ</t>
-  </si>
-  <si>
-    <t>1D863</t>
   </si>
   <si>
     <t>ែ</t>
   </si>
   <si>
-    <t>1D864</t>
-  </si>
-  <si>
     <t>ៃ</t>
-  </si>
-  <si>
-    <t>1D865</t>
   </si>
   <si>
     <t>ោ</t>
   </si>
   <si>
-    <t>1D868</t>
-  </si>
-  <si>
     <t>ៅ</t>
-  </si>
-  <si>
-    <t>1D867</t>
   </si>
   <si>
     <t>ុំ</t>
   </si>
   <si>
-    <t>1D825</t>
-  </si>
-  <si>
     <t>ំ</t>
-  </si>
-  <si>
-    <t>1D91C</t>
   </si>
   <si>
     <t>ាំ</t>
@@ -351,187 +198,79 @@
     <t>ះ</t>
   </si>
   <si>
-    <t>1D823</t>
-  </si>
-  <si>
     <t>ុះ</t>
-  </si>
-  <si>
-    <t>1D824</t>
   </si>
   <si>
     <t>េះ</t>
   </si>
   <si>
-    <t>1D91F</t>
-  </si>
-  <si>
     <t>ោះ</t>
-  </si>
-  <si>
-    <t>1D91A</t>
   </si>
   <si>
     <t>ឥ</t>
   </si>
   <si>
-    <t>1D8E4</t>
-  </si>
-  <si>
     <t>ឦ</t>
-  </si>
-  <si>
-    <t>1D8E5</t>
   </si>
   <si>
     <t>ឧ</t>
   </si>
   <si>
-    <t>1D8E6</t>
-  </si>
-  <si>
     <t>ឩ</t>
-  </si>
-  <si>
-    <t>1D8E7</t>
   </si>
   <si>
     <t>ឪ</t>
   </si>
   <si>
-    <t>1D8E9</t>
-  </si>
-  <si>
     <t>ឫ</t>
-  </si>
-  <si>
-    <t>1D8EC</t>
   </si>
   <si>
     <t>ឬ</t>
   </si>
   <si>
-    <t>1d8ED</t>
-  </si>
-  <si>
     <t>ឭ</t>
-  </si>
-  <si>
-    <t>1D8BB</t>
   </si>
   <si>
     <t>ឮ</t>
   </si>
   <si>
-    <t>1D8BC</t>
-  </si>
-  <si>
     <t>ឯ</t>
-  </si>
-  <si>
-    <t>1D8AA</t>
   </si>
   <si>
     <t>ឰ</t>
   </si>
   <si>
-    <t>1D8BD</t>
-  </si>
-  <si>
     <t>ឱ</t>
-  </si>
-  <si>
-    <t>1D8E8</t>
   </si>
   <si>
     <t>ឲ</t>
   </si>
   <si>
-    <t>1D8CF</t>
-  </si>
-  <si>
     <t>៊</t>
-  </si>
-  <si>
-    <t>1D9DA</t>
   </si>
   <si>
     <t>៉</t>
   </si>
   <si>
-    <t>1D928</t>
-  </si>
-  <si>
     <t>៌</t>
-  </si>
-  <si>
-    <t>1D910</t>
   </si>
   <si>
     <t>់</t>
   </si>
   <si>
-    <t>1D929</t>
-  </si>
-  <si>
     <t>៍</t>
-  </si>
-  <si>
-    <t>1D911</t>
   </si>
   <si>
     <t>័</t>
   </si>
   <si>
-    <t>1D914</t>
-  </si>
-  <si>
     <t>៏</t>
-  </si>
-  <si>
-    <t>1D915</t>
   </si>
   <si>
     <t>៎</t>
   </si>
   <si>
-    <t>1D908</t>
-  </si>
-  <si>
     <t>ៈ</t>
-  </si>
-  <si>
-    <t>1D919</t>
-  </si>
-  <si>
-    <t>1D875</t>
-  </si>
-  <si>
-    <t>1D8A1</t>
-  </si>
-  <si>
-    <t>1D8A5</t>
-  </si>
-  <si>
-    <t>1D859</t>
-  </si>
-  <si>
-    <t>1D857</t>
-  </si>
-  <si>
-    <t>1D8B8</t>
-  </si>
-  <si>
-    <t>1D8DD</t>
-  </si>
-  <si>
-    <t>1D89D</t>
-  </si>
-  <si>
-    <t>1D858</t>
-  </si>
-  <si>
-    <t>1D876</t>
   </si>
   <si>
     <t>ឡ</t>
@@ -552,14 +291,281 @@
     <t>៚</t>
   </si>
   <si>
-    <t>1D82D</t>
+    <t>U+1D873</t>
+  </si>
+  <si>
+    <t>U+1D806</t>
+  </si>
+  <si>
+    <t>U+1D816</t>
+  </si>
+  <si>
+    <t>U+1D8A4</t>
+  </si>
+  <si>
+    <t>U+1D842</t>
+  </si>
+  <si>
+    <t>U+1D845</t>
+  </si>
+  <si>
+    <t>U+1D850</t>
+  </si>
+  <si>
+    <t>U+1D8B4</t>
+  </si>
+  <si>
+    <t>U+1D834</t>
+  </si>
+  <si>
+    <t>U+1D893</t>
+  </si>
+  <si>
+    <t>U+1D8CC</t>
+  </si>
+  <si>
+    <t>U+1D8C6</t>
+  </si>
+  <si>
+    <t>U+1D829</t>
+  </si>
+  <si>
+    <t>U+1D8BA</t>
+  </si>
+  <si>
+    <t>U+1D8EF</t>
+  </si>
+  <si>
+    <t>U+1D84A</t>
+  </si>
+  <si>
+    <t>U+1D89C</t>
+  </si>
+  <si>
+    <t>U+1D83E</t>
+  </si>
+  <si>
+    <t>U+1D844</t>
+  </si>
+  <si>
+    <t>U+1D895</t>
+  </si>
+  <si>
+    <t>U+1D8A0</t>
+  </si>
+  <si>
+    <t>U+1D813</t>
+  </si>
+  <si>
+    <t>U+1D846</t>
+  </si>
+  <si>
+    <t>U+1D828</t>
+  </si>
+  <si>
+    <t>U+1D848</t>
+  </si>
+  <si>
+    <t>U+1D88C</t>
+  </si>
+  <si>
+    <t>U+1D81D</t>
+  </si>
+  <si>
+    <t>U+1D82C</t>
+  </si>
+  <si>
+    <t>U+1D82E</t>
+  </si>
+  <si>
+    <t>U+1D896</t>
+  </si>
+  <si>
+    <t>U+1D898</t>
+  </si>
+  <si>
+    <t>U+1D8C4</t>
+  </si>
+  <si>
+    <t>U+1D8B5</t>
+  </si>
+  <si>
+    <t>U+1D879</t>
+  </si>
+  <si>
+    <t>U+1D85C</t>
+  </si>
+  <si>
+    <t>U+1D85E</t>
+  </si>
+  <si>
+    <t>U+1D809</t>
+  </si>
+  <si>
+    <t>U+1D819</t>
+  </si>
+  <si>
+    <t>U+1D8C8</t>
+  </si>
+  <si>
+    <t>U+1D8C9</t>
+  </si>
+  <si>
+    <t>U+1D8CB</t>
+  </si>
+  <si>
+    <t>U+1D87F</t>
+  </si>
+  <si>
+    <t>U+1D86A</t>
+  </si>
+  <si>
+    <t>U+1D869</t>
+  </si>
+  <si>
+    <t>U+1D863</t>
+  </si>
+  <si>
+    <t>U+1D864</t>
+  </si>
+  <si>
+    <t>U+1D865</t>
+  </si>
+  <si>
+    <t>U+1D868</t>
+  </si>
+  <si>
+    <t>U+1D867</t>
+  </si>
+  <si>
+    <t>U+1D825</t>
+  </si>
+  <si>
+    <t>U+1D91C</t>
+  </si>
+  <si>
+    <t>U+1D823</t>
+  </si>
+  <si>
+    <t>U+1D824</t>
+  </si>
+  <si>
+    <t>U+1D91F</t>
+  </si>
+  <si>
+    <t>U+1D91A</t>
+  </si>
+  <si>
+    <t>U+1D8E4</t>
+  </si>
+  <si>
+    <t>U+1D8E5</t>
+  </si>
+  <si>
+    <t>U+1D8E6</t>
+  </si>
+  <si>
+    <t>U+1D8E7</t>
+  </si>
+  <si>
+    <t>U+1D8E9</t>
+  </si>
+  <si>
+    <t>U+1D8EC</t>
+  </si>
+  <si>
+    <t>U+1d8ED</t>
+  </si>
+  <si>
+    <t>U+1D8BB</t>
+  </si>
+  <si>
+    <t>U+1D8BC</t>
+  </si>
+  <si>
+    <t>U+1D8AA</t>
+  </si>
+  <si>
+    <t>U+1D8BD</t>
+  </si>
+  <si>
+    <t>U+1D8E8</t>
+  </si>
+  <si>
+    <t>U+1D8CF</t>
+  </si>
+  <si>
+    <t>U+1D9DA</t>
+  </si>
+  <si>
+    <t>U+1D928</t>
+  </si>
+  <si>
+    <t>U+1D910</t>
+  </si>
+  <si>
+    <t>U+1D929</t>
+  </si>
+  <si>
+    <t>U+1D911</t>
+  </si>
+  <si>
+    <t>U+1D914</t>
+  </si>
+  <si>
+    <t>U+1D915</t>
+  </si>
+  <si>
+    <t>U+1D908</t>
+  </si>
+  <si>
+    <t>U+1D919</t>
+  </si>
+  <si>
+    <t>U+1D875</t>
+  </si>
+  <si>
+    <t>U+1D8A1</t>
+  </si>
+  <si>
+    <t>U+1D8A5</t>
+  </si>
+  <si>
+    <t>U+1D859</t>
+  </si>
+  <si>
+    <t>U+1D857</t>
+  </si>
+  <si>
+    <t>U+1D8B8</t>
+  </si>
+  <si>
+    <t>U+1D8DD</t>
+  </si>
+  <si>
+    <t>U+1D89D</t>
+  </si>
+  <si>
+    <t>U+1D858</t>
+  </si>
+  <si>
+    <t>U+1D876</t>
+  </si>
+  <si>
+    <t>U+1D82D</t>
+  </si>
+  <si>
+    <t>្</t>
+  </si>
+  <si>
+    <t>U+1D93E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -600,6 +606,21 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Liberation sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Liberation sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Liberation sans"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -708,7 +729,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -773,19 +794,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1003,18 +1027,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B86" zoomScale="252" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
     <col min="2" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="5" max="5" width="53.1640625" customWidth="1"/>
-    <col min="6" max="6" width="8.5" customWidth="1"/>
-    <col min="7" max="26" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="53.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="31.5" customHeight="1">
@@ -1063,7 +1087,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7"/>
@@ -1093,10 +1117,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>8</v>
+        <v>89</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
@@ -1126,10 +1150,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="7"/>
@@ -1159,11 +1183,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="5" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
@@ -1193,11 +1217,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
@@ -1227,11 +1251,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="5" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
@@ -1261,11 +1285,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="5" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
@@ -1295,11 +1319,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="5" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
@@ -1329,11 +1353,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="5" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="7"/>
@@ -1363,11 +1387,11 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="5" t="s">
-        <v>24</v>
+        <v>97</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
@@ -1397,11 +1421,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="5" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="7"/>
@@ -1431,11 +1455,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="5" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="7"/>
@@ -1465,11 +1489,11 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="5" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="7"/>
@@ -1499,11 +1523,11 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="5" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
@@ -1533,11 +1557,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="5" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
@@ -1567,11 +1591,11 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="5" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="7"/>
@@ -1601,11 +1625,11 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="5" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
@@ -1635,11 +1659,11 @@
         <v>18</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="5" t="s">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
@@ -1669,11 +1693,11 @@
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="5" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="7"/>
@@ -1703,11 +1727,11 @@
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="5" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="7"/>
@@ -1737,11 +1761,11 @@
         <v>21</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="5" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="7"/>
@@ -1771,11 +1795,11 @@
         <v>22</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="5" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="7"/>
@@ -1805,11 +1829,11 @@
         <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="5" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="7"/>
@@ -1839,11 +1863,11 @@
         <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="5" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="7"/>
@@ -1873,11 +1897,11 @@
         <v>25</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="5" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="7"/>
@@ -1907,11 +1931,11 @@
         <v>26</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="5" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="7"/>
@@ -1941,11 +1965,11 @@
         <v>27</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="5" t="s">
-        <v>58</v>
+        <v>114</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="7"/>
@@ -1975,11 +1999,11 @@
         <v>28</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="5" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="7"/>
@@ -2009,11 +2033,11 @@
         <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="5" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="7"/>
@@ -2043,11 +2067,11 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="5" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="7"/>
@@ -2077,11 +2101,11 @@
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="5" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="7"/>
@@ -2111,11 +2135,11 @@
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="5" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="7"/>
@@ -2145,11 +2169,11 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="5" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="7"/>
@@ -2179,11 +2203,11 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="5" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="7"/>
@@ -2213,11 +2237,11 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="5" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="7"/>
@@ -2247,11 +2271,11 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="5" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="7"/>
@@ -2281,11 +2305,11 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="5" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="7"/>
@@ -2315,11 +2339,11 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="5" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="7"/>
@@ -2349,11 +2373,11 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="5" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="7"/>
@@ -2383,11 +2407,11 @@
         <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="5" t="s">
-        <v>83</v>
+        <v>127</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="7"/>
@@ -2417,11 +2441,11 @@
         <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="5" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="7"/>
@@ -2451,11 +2475,11 @@
         <v>42</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="5" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="7"/>
@@ -2485,11 +2509,11 @@
         <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="5" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="7"/>
@@ -2519,11 +2543,11 @@
         <v>44</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="5" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="7"/>
@@ -2553,11 +2577,11 @@
         <v>45</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="5" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="7"/>
@@ -2587,11 +2611,11 @@
         <v>46</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="5" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="7"/>
@@ -2621,11 +2645,11 @@
         <v>47</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="5" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="7"/>
@@ -2655,11 +2679,11 @@
         <v>48</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="5" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="7"/>
@@ -2689,11 +2713,11 @@
         <v>49</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="C50" s="9"/>
       <c r="D50" s="5" t="s">
-        <v>101</v>
+        <v>136</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="7"/>
@@ -2723,11 +2747,11 @@
         <v>50</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="5" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="7"/>
@@ -2757,11 +2781,11 @@
         <v>51</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="5" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="E52" s="6"/>
       <c r="F52" s="7"/>
@@ -2791,11 +2815,11 @@
         <v>52</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="C53" s="9"/>
       <c r="D53" s="5" t="s">
-        <v>101</v>
+        <v>136</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="7"/>
@@ -2825,11 +2849,11 @@
         <v>53</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="5" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="7"/>
@@ -2859,11 +2883,11 @@
         <v>54</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="C55" s="9"/>
       <c r="D55" s="5" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="E55" s="6"/>
       <c r="F55" s="7"/>
@@ -2893,11 +2917,11 @@
         <v>55</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="5" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="E56" s="6"/>
       <c r="F56" s="7"/>
@@ -2927,11 +2951,11 @@
         <v>56</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>113</v>
+        <v>59</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="5" t="s">
-        <v>114</v>
+        <v>142</v>
       </c>
       <c r="E57" s="6"/>
       <c r="F57" s="7"/>
@@ -2961,11 +2985,11 @@
         <v>57</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="E58" s="6"/>
       <c r="F58" s="7"/>
@@ -2995,11 +3019,11 @@
         <v>58</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
       <c r="C59" s="5"/>
-      <c r="D59" s="5" t="s">
-        <v>118</v>
+      <c r="D59" s="29" t="s">
+        <v>144</v>
       </c>
       <c r="E59" s="6"/>
       <c r="F59" s="7"/>
@@ -3029,11 +3053,11 @@
         <v>59</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>119</v>
+        <v>62</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="5" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="E60" s="6"/>
       <c r="F60" s="7"/>
@@ -3063,11 +3087,11 @@
         <v>60</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="C61" s="5"/>
-      <c r="D61" s="5" t="s">
-        <v>122</v>
+      <c r="D61" s="29" t="s">
+        <v>146</v>
       </c>
       <c r="E61" s="6"/>
       <c r="F61" s="7"/>
@@ -3097,11 +3121,11 @@
         <v>61</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>123</v>
+        <v>64</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="7"/>
@@ -3131,11 +3155,11 @@
         <v>62</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="E63" s="6"/>
       <c r="F63" s="7"/>
@@ -3165,11 +3189,11 @@
         <v>63</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>127</v>
+        <v>66</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="E64" s="6"/>
       <c r="F64" s="7"/>
@@ -3199,11 +3223,11 @@
         <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="E65" s="6"/>
       <c r="F65" s="7"/>
@@ -3233,11 +3257,11 @@
         <v>65</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>131</v>
+        <v>68</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="E66" s="6"/>
       <c r="F66" s="7"/>
@@ -3267,11 +3291,11 @@
         <v>66</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="E67" s="6"/>
       <c r="F67" s="7"/>
@@ -3301,11 +3325,11 @@
         <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="E68" s="6"/>
       <c r="F68" s="7"/>
@@ -3335,11 +3359,11 @@
         <v>68</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>137</v>
+        <v>71</v>
       </c>
       <c r="C69" s="5"/>
-      <c r="D69" s="5" t="s">
-        <v>138</v>
+      <c r="D69" s="28" t="s">
+        <v>154</v>
       </c>
       <c r="E69" s="6"/>
       <c r="F69" s="7"/>
@@ -3369,11 +3393,11 @@
         <v>69</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>139</v>
+        <v>72</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="E70" s="6"/>
       <c r="F70" s="7"/>
@@ -3403,11 +3427,11 @@
         <v>70</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="E71" s="6"/>
       <c r="F71" s="7"/>
@@ -3437,11 +3461,11 @@
         <v>71</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>143</v>
+        <v>74</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="E72" s="6"/>
       <c r="F72" s="7"/>
@@ -3471,11 +3495,11 @@
         <v>72</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>145</v>
+        <v>75</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="5" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="E73" s="6"/>
       <c r="F73" s="7"/>
@@ -3505,11 +3529,11 @@
         <v>73</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>147</v>
+        <v>76</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="E74" s="6"/>
       <c r="F74" s="7"/>
@@ -3539,11 +3563,11 @@
         <v>74</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>149</v>
+        <v>77</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="E75" s="6"/>
       <c r="F75" s="7"/>
@@ -3573,11 +3597,11 @@
         <v>75</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>151</v>
+        <v>78</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="E76" s="6"/>
       <c r="F76" s="7"/>
@@ -3607,11 +3631,11 @@
         <v>76</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>153</v>
+        <v>79</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="E77" s="6"/>
       <c r="F77" s="7"/>
@@ -3641,11 +3665,11 @@
         <v>77</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E78" s="6"/>
       <c r="F78" s="7"/>
@@ -3675,11 +3699,11 @@
         <v>78</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="E79" s="6"/>
       <c r="F79" s="7"/>
@@ -3713,7 +3737,7 @@
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="E80" s="6"/>
       <c r="F80" s="7"/>
@@ -3747,7 +3771,7 @@
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E81" s="6"/>
       <c r="F81" s="7"/>
@@ -3781,7 +3805,7 @@
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="E82" s="6"/>
       <c r="F82" s="7"/>
@@ -3815,7 +3839,7 @@
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="E83" s="6"/>
       <c r="F83" s="7"/>
@@ -3849,7 +3873,7 @@
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="E84" s="6"/>
       <c r="F84" s="7"/>
@@ -3883,7 +3907,7 @@
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="5" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="E85" s="6"/>
       <c r="F85" s="7"/>
@@ -3917,7 +3941,7 @@
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="5" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="E86" s="6"/>
       <c r="F86" s="7"/>
@@ -3951,7 +3975,7 @@
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="5" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="E87" s="6"/>
       <c r="F87" s="7"/>
@@ -3985,7 +4009,7 @@
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="5" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="E88" s="6"/>
       <c r="F88" s="7"/>
@@ -4019,7 +4043,7 @@
       </c>
       <c r="C89" s="18"/>
       <c r="D89" s="18" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="E89" s="19"/>
       <c r="F89" s="7"/>
@@ -4049,11 +4073,11 @@
         <v>89</v>
       </c>
       <c r="B90" s="23" t="s">
-        <v>169</v>
+        <v>82</v>
       </c>
       <c r="C90" s="24"/>
       <c r="D90" s="24" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="E90" s="25"/>
       <c r="F90" s="7"/>
@@ -4083,7 +4107,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="23" t="s">
-        <v>170</v>
+        <v>83</v>
       </c>
       <c r="C91" s="24"/>
       <c r="D91" s="24" t="s">
@@ -4117,7 +4141,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="23" t="s">
-        <v>172</v>
+        <v>85</v>
       </c>
       <c r="C92" s="24"/>
       <c r="D92" s="24"/>
@@ -4149,7 +4173,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="23" t="s">
-        <v>173</v>
+        <v>86</v>
       </c>
       <c r="C93" s="24"/>
       <c r="D93" s="24"/>
@@ -4181,7 +4205,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="23" t="s">
-        <v>174</v>
+        <v>87</v>
       </c>
       <c r="C94" s="24"/>
       <c r="D94" s="24"/>
@@ -4212,8 +4236,8 @@
       <c r="A95" s="22">
         <v>94</v>
       </c>
-      <c r="B95" s="26" t="s">
-        <v>171</v>
+      <c r="B95" s="23" t="s">
+        <v>84</v>
       </c>
       <c r="C95" s="24"/>
       <c r="D95" s="24"/>
@@ -4241,10 +4265,14 @@
       <c r="Z95" s="7"/>
     </row>
     <row r="96" spans="1:26" ht="31.5" customHeight="1">
-      <c r="A96" s="30"/>
-      <c r="B96" s="27"/>
+      <c r="A96" s="27"/>
+      <c r="B96" s="30" t="s">
+        <v>176</v>
+      </c>
       <c r="C96" s="20"/>
-      <c r="D96" s="20"/>
+      <c r="D96" s="31" t="s">
+        <v>177</v>
+      </c>
       <c r="E96" s="21"/>
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
@@ -4269,8 +4297,8 @@
       <c r="Z96" s="7"/>
     </row>
     <row r="97" spans="1:26" ht="31.5" customHeight="1">
-      <c r="A97" s="30"/>
-      <c r="B97" s="28"/>
+      <c r="A97" s="27"/>
+      <c r="B97" s="26"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="7"/>
@@ -4297,8 +4325,8 @@
       <c r="Z97" s="7"/>
     </row>
     <row r="98" spans="1:26" ht="31.5" customHeight="1">
-      <c r="A98" s="30"/>
-      <c r="B98" s="28"/>
+      <c r="A98" s="27"/>
+      <c r="B98" s="26"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
       <c r="E98" s="7"/>
@@ -4325,8 +4353,8 @@
       <c r="Z98" s="7"/>
     </row>
     <row r="99" spans="1:26" ht="31.5" customHeight="1">
-      <c r="A99" s="30"/>
-      <c r="B99" s="28"/>
+      <c r="A99" s="27"/>
+      <c r="B99" s="26"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="7"/>
@@ -4354,7 +4382,7 @@
     </row>
     <row r="100" spans="1:26" ht="31.5" customHeight="1">
       <c r="A100" s="16"/>
-      <c r="B100" s="29"/>
+      <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="7"/>
@@ -29582,7 +29610,7 @@
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370000000000011" bottom="0.39370000000000011" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>